<commit_message>
Added validation rules to ExecTime column
Now only allow whole numbers 0-999 to be entered.  Message added indicating this and not to enter "m".  Error occurs if data validation rule broken.  Avoids scenario as reported by Ana Paula Olvia (thank you for bug report Ana!)
</commit_message>
<xml_diff>
--- a/download/my_test_case_manager.xlsx
+++ b/download/my_test_case_manager.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCC1211-9492-4A67-907F-A7AB576B9D49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6FBFA6-EF2E-4EB7-89FA-7A6711A48935}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="19416" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="36" r:id="rId1"/>
@@ -283,9 +283,6 @@
     <t>Release Notes</t>
   </si>
   <si>
-    <t xml:space="preserve"> v5.01.44299</t>
-  </si>
-  <si>
     <t>Add "Release Notes" tab to templates (not samples).  Date and version stamp each release.  Number the fixes.</t>
   </si>
   <si>
@@ -320,6 +317,9 @@
   </si>
   <si>
     <t>Releasability Graph allows for 0.5 in the count when count is low (integer only).  Check all graphs…confirmed most are wrong, especially when no data.  Fix all by setting minimum graph unit to 1, while leaving max to Auto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> v5.01.44308</t>
   </si>
 </sst>
 </file>
@@ -9375,7 +9375,7 @@
   <dimension ref="A1:L320"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12765,9 +12765,13 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="   - (Press delete to clear)_x000a_i  - Information_x000a_T - To Do_x000a_B - Blocked_x000a_F - Fail_x000a_Q - Qualified Pass_x000a_P - Pass" sqref="D19:D318" xr:uid="{82A7EADB-1480-405F-AB2E-6962FBFFF165}">
       <formula1>"i,T,B,F,Q,P"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter time in minutes (0-999)" prompt="Do no enter the &quot;m&quot;." sqref="C19:C318" xr:uid="{DDF9A720-D7EF-4D6B-87E6-3914070F8D73}">
+      <formula1>0</formula1>
+      <formula2>999</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13991,7 +13995,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14041,7 +14045,7 @@
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="3" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="12"/>
@@ -14068,10 +14072,10 @@
       <c r="A7" s="59"/>
       <c r="B7" s="59"/>
       <c r="C7" s="113" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D7" s="159" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" s="159"/>
       <c r="F7" s="159"/>
@@ -14081,7 +14085,7 @@
       <c r="A8" s="59"/>
       <c r="B8" s="59"/>
       <c r="C8" s="113" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8" s="160" t="s">
         <v>51</v>
@@ -14094,10 +14098,10 @@
       <c r="A9" s="59"/>
       <c r="B9" s="59"/>
       <c r="C9" s="113" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="159" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9" s="160"/>
       <c r="F9" s="160"/>
@@ -14209,7 +14213,7 @@
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E21" s="120">
         <f ca="1">TODAY()</f>
-        <v>44299</v>
+        <v>44308</v>
       </c>
       <c r="F21" s="120"/>
     </row>
@@ -14274,7 +14278,7 @@
     <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="54"/>
       <c r="B4" s="161" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="161"/>
       <c r="D4" s="54"/>
@@ -14285,7 +14289,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="137" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5" s="54"/>
     </row>
@@ -14295,7 +14299,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="137" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" s="54"/>
     </row>
@@ -14305,7 +14309,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="137" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" s="54"/>
     </row>
@@ -14315,7 +14319,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="137" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" s="54"/>
     </row>
@@ -14325,7 +14329,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="137" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" s="54"/>
     </row>
@@ -14335,7 +14339,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="137" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" s="54"/>
     </row>

</xml_diff>

<commit_message>
Forgot to update the release notes tab
So added the fix notes in now for recent release.
</commit_message>
<xml_diff>
--- a/download/my_test_case_manager.xlsx
+++ b/download/my_test_case_manager.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6FBFA6-EF2E-4EB7-89FA-7A6711A48935}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8388C1E2-6046-4CC5-B378-56B06D991ED7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="19416" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="36" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="74">
   <si>
     <t>F</t>
   </si>
@@ -283,21 +283,6 @@
     <t>Release Notes</t>
   </si>
   <si>
-    <t>Add "Release Notes" tab to templates (not samples).  Date and version stamp each release.  Number the fixes.</t>
-  </si>
-  <si>
-    <t>Add a link to the Basic XL YouTube PlayList to offer free training on Excel usage tips</t>
-  </si>
-  <si>
-    <t>Defect trend graph Open has border turned on for red (should be fill only) check all</t>
-  </si>
-  <si>
-    <t>v5.01.44299  -  4/13/2021</t>
-  </si>
-  <si>
-    <t>Make About screen point to YouTube PlayList, not the overall site link</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/playlist?list=PLVHoUDdbskUSZQsl0iexHwRGb8Z7_EjlS</t>
   </si>
   <si>
@@ -313,13 +298,35 @@
     <t>https://www.youtube.com/playlist?list=PLVHoUDdbskUQXl0S6nS2QUMB69rrf1zcF</t>
   </si>
   <si>
-    <t>Re-order graph series so that Qpass is adjacent to Pass in all Test Case count and trend graphs (at least one is wrong)</t>
+    <t xml:space="preserve"> v5.01.44308</t>
   </si>
   <si>
-    <t>Releasability Graph allows for 0.5 in the count when count is low (integer only).  Check all graphs…confirmed most are wrong, especially when no data.  Fix all by setting minimum graph unit to 1, while leaving max to Auto.</t>
+    <t>v5.01.44299  -  2021.04.13</t>
   </si>
   <si>
-    <t xml:space="preserve"> v5.01.44308</t>
+    <t>v5.01.44308  -  202104.22</t>
+  </si>
+  <si>
+    <t>CHANGE - Add "Release Notes" tab to templates (not samples).  Date and version stamp each release.  Number the fixes.</t>
+  </si>
+  <si>
+    <t>CHANGE - Make About screen point to YouTube PlayList, not the overall site link</t>
+  </si>
+  <si>
+    <t>CHANGE - Add a link to the Basic XL YouTube PlayList to offer free training on Excel usage tips</t>
+  </si>
+  <si>
+    <t>DEFECT - Re-order graph series so that Qpass is adjacent to Pass in all Test Case count and trend graphs (at least one is wrong)</t>
+  </si>
+  <si>
+    <t>DEFECT - Trend graph Open has border turned on for red (should be fill only) check all</t>
+  </si>
+  <si>
+    <t>DEFECT - Releasability Graph allows for 0.5 in the count when count is low (integer only).  Check all graphs…confirmed most are wrong, especially when no data.  Fix all by setting minimum graph unit to 1, while leaving max to Auto.</t>
+  </si>
+  <si>
+    <t>DEFECT - Now only allow whole numbers 0-999 to be entered. Message added indicating this and not to enter "m".
+Error occurs if data validation rule broken. Avoids scenario as reported by Ana Paula Olvia (thank you for bug report Ana!)</t>
   </si>
 </sst>
 </file>
@@ -1446,14 +1453,14 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1470,14 +1477,14 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -13049,44 +13056,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" s="93" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="B1" s="155" t="s">
+      <c r="B1" s="147" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="155"/>
-      <c r="D1" s="155"/>
-      <c r="E1" s="155"/>
-      <c r="F1" s="155"/>
-      <c r="G1" s="155"/>
-      <c r="H1" s="155"/>
-      <c r="I1" s="155"/>
-      <c r="J1" s="155"/>
-      <c r="K1" s="155"/>
-      <c r="L1" s="155"/>
-      <c r="M1" s="155"/>
-      <c r="N1" s="155"/>
-      <c r="O1" s="155"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="147"/>
+      <c r="H1" s="147"/>
+      <c r="I1" s="147"/>
+      <c r="J1" s="147"/>
+      <c r="K1" s="147"/>
+      <c r="L1" s="147"/>
+      <c r="M1" s="147"/>
+      <c r="N1" s="147"/>
+      <c r="O1" s="147"/>
       <c r="Q1" s="94"/>
     </row>
     <row r="2" spans="2:17" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C2" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="154" t="str">
+      <c r="D2" s="146" t="str">
         <f>IF(Properties!$C$4=0, "", Properties!$C$4)</f>
         <v/>
       </c>
-      <c r="E2" s="154"/>
-      <c r="F2" s="154"/>
-      <c r="G2" s="154"/>
-      <c r="H2" s="154"/>
+      <c r="E2" s="146"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="146"/>
       <c r="M2" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="153" t="str" cm="1">
+      <c r="N2" s="145" t="str" cm="1">
         <f t="array" ref="N2">INDEX('Test Run Log'!$B$5:$B$6,MATCH(MAX(COUNTIF('Test Run Log'!$B$5:$B$6, "&lt;" &amp; 'Test Run Log'!$B$5:$B$6)), COUNTIF('Test Run Log'!$B$5:$B$6, "&lt;"&amp;'Test Run Log'!$B$5:$B$6),0))</f>
         <v>R2</v>
       </c>
-      <c r="O2" s="153"/>
+      <c r="O2" s="145"/>
       <c r="Q2" s="95"/>
     </row>
     <row r="3" spans="2:17" s="57" customFormat="1" x14ac:dyDescent="0.3">
@@ -13094,22 +13101,22 @@
       <c r="C3" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="153" t="str">
+      <c r="D3" s="145" t="str">
         <f>IF(Properties!$C$6=0, "", Properties!$C$6)</f>
         <v/>
       </c>
-      <c r="E3" s="153"/>
-      <c r="F3" s="153"/>
-      <c r="G3" s="153"/>
-      <c r="H3" s="153"/>
+      <c r="E3" s="145"/>
+      <c r="F3" s="145"/>
+      <c r="G3" s="145"/>
+      <c r="H3" s="145"/>
       <c r="M3" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="153" t="str">
+      <c r="N3" s="145" t="str">
         <f>IF(Properties!$C$8=0, "", Properties!$C$8)</f>
         <v/>
       </c>
-      <c r="O3" s="153"/>
+      <c r="O3" s="145"/>
       <c r="Q3" s="95"/>
     </row>
     <row r="4" spans="2:17" s="57" customFormat="1" x14ac:dyDescent="0.3">
@@ -13119,11 +13126,11 @@
       <c r="M4" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="N4" s="154">
+      <c r="N4" s="146">
         <f>SUM(C14:G14)</f>
         <v>0</v>
       </c>
-      <c r="O4" s="154"/>
+      <c r="O4" s="146"/>
       <c r="Q4" s="95"/>
     </row>
     <row r="5" spans="2:17" s="57" customFormat="1" x14ac:dyDescent="0.3">
@@ -13133,11 +13140,11 @@
       <c r="M5" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="N5" s="154">
+      <c r="N5" s="146">
         <f>SUM(K14:M14)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="154"/>
+      <c r="O5" s="146"/>
       <c r="Q5" s="95"/>
     </row>
     <row r="6" spans="2:17" ht="6.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -13551,85 +13558,85 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B44" s="116"/>
-      <c r="C44" s="145"/>
-      <c r="D44" s="146"/>
-      <c r="E44" s="146"/>
-      <c r="F44" s="146"/>
-      <c r="G44" s="146"/>
-      <c r="H44" s="146"/>
-      <c r="I44" s="146"/>
-      <c r="J44" s="146"/>
-      <c r="K44" s="146"/>
-      <c r="L44" s="146"/>
-      <c r="M44" s="146"/>
-      <c r="N44" s="146"/>
-      <c r="O44" s="147"/>
+      <c r="C44" s="153"/>
+      <c r="D44" s="154"/>
+      <c r="E44" s="154"/>
+      <c r="F44" s="154"/>
+      <c r="G44" s="154"/>
+      <c r="H44" s="154"/>
+      <c r="I44" s="154"/>
+      <c r="J44" s="154"/>
+      <c r="K44" s="154"/>
+      <c r="L44" s="154"/>
+      <c r="M44" s="154"/>
+      <c r="N44" s="154"/>
+      <c r="O44" s="155"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B45" s="116"/>
-      <c r="C45" s="145"/>
-      <c r="D45" s="146"/>
-      <c r="E45" s="146"/>
-      <c r="F45" s="146"/>
-      <c r="G45" s="146"/>
-      <c r="H45" s="146"/>
-      <c r="I45" s="146"/>
-      <c r="J45" s="146"/>
-      <c r="K45" s="146"/>
-      <c r="L45" s="146"/>
-      <c r="M45" s="146"/>
-      <c r="N45" s="146"/>
-      <c r="O45" s="147"/>
+      <c r="C45" s="153"/>
+      <c r="D45" s="154"/>
+      <c r="E45" s="154"/>
+      <c r="F45" s="154"/>
+      <c r="G45" s="154"/>
+      <c r="H45" s="154"/>
+      <c r="I45" s="154"/>
+      <c r="J45" s="154"/>
+      <c r="K45" s="154"/>
+      <c r="L45" s="154"/>
+      <c r="M45" s="154"/>
+      <c r="N45" s="154"/>
+      <c r="O45" s="155"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B46" s="116"/>
-      <c r="C46" s="145"/>
-      <c r="D46" s="146"/>
-      <c r="E46" s="146"/>
-      <c r="F46" s="146"/>
-      <c r="G46" s="146"/>
-      <c r="H46" s="146"/>
-      <c r="I46" s="146"/>
-      <c r="J46" s="146"/>
-      <c r="K46" s="146"/>
-      <c r="L46" s="146"/>
-      <c r="M46" s="146"/>
-      <c r="N46" s="146"/>
-      <c r="O46" s="147"/>
+      <c r="C46" s="153"/>
+      <c r="D46" s="154"/>
+      <c r="E46" s="154"/>
+      <c r="F46" s="154"/>
+      <c r="G46" s="154"/>
+      <c r="H46" s="154"/>
+      <c r="I46" s="154"/>
+      <c r="J46" s="154"/>
+      <c r="K46" s="154"/>
+      <c r="L46" s="154"/>
+      <c r="M46" s="154"/>
+      <c r="N46" s="154"/>
+      <c r="O46" s="155"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
       <c r="B47" s="118"/>
-      <c r="C47" s="145"/>
-      <c r="D47" s="146"/>
-      <c r="E47" s="146"/>
-      <c r="F47" s="146"/>
-      <c r="G47" s="146"/>
-      <c r="H47" s="146"/>
-      <c r="I47" s="146"/>
-      <c r="J47" s="146"/>
-      <c r="K47" s="146"/>
-      <c r="L47" s="146"/>
-      <c r="M47" s="146"/>
-      <c r="N47" s="146"/>
-      <c r="O47" s="147"/>
+      <c r="C47" s="153"/>
+      <c r="D47" s="154"/>
+      <c r="E47" s="154"/>
+      <c r="F47" s="154"/>
+      <c r="G47" s="154"/>
+      <c r="H47" s="154"/>
+      <c r="I47" s="154"/>
+      <c r="J47" s="154"/>
+      <c r="K47" s="154"/>
+      <c r="L47" s="154"/>
+      <c r="M47" s="154"/>
+      <c r="N47" s="154"/>
+      <c r="O47" s="155"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="10"/>
       <c r="B48" s="117"/>
-      <c r="C48" s="145"/>
-      <c r="D48" s="146"/>
-      <c r="E48" s="146"/>
-      <c r="F48" s="146"/>
-      <c r="G48" s="146"/>
-      <c r="H48" s="146"/>
-      <c r="I48" s="146"/>
-      <c r="J48" s="146"/>
-      <c r="K48" s="146"/>
-      <c r="L48" s="146"/>
-      <c r="M48" s="146"/>
-      <c r="N48" s="146"/>
-      <c r="O48" s="147"/>
+      <c r="C48" s="153"/>
+      <c r="D48" s="154"/>
+      <c r="E48" s="154"/>
+      <c r="F48" s="154"/>
+      <c r="G48" s="154"/>
+      <c r="H48" s="154"/>
+      <c r="I48" s="154"/>
+      <c r="J48" s="154"/>
+      <c r="K48" s="154"/>
+      <c r="L48" s="154"/>
+      <c r="M48" s="154"/>
+      <c r="N48" s="154"/>
+      <c r="O48" s="155"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
@@ -13677,89 +13684,89 @@
     </row>
     <row r="52" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B52" s="116"/>
-      <c r="C52" s="145"/>
-      <c r="D52" s="146"/>
-      <c r="E52" s="146"/>
-      <c r="F52" s="146"/>
-      <c r="G52" s="146"/>
-      <c r="H52" s="146"/>
-      <c r="I52" s="146"/>
-      <c r="J52" s="146"/>
-      <c r="K52" s="146"/>
-      <c r="L52" s="146"/>
-      <c r="M52" s="146"/>
-      <c r="N52" s="146"/>
-      <c r="O52" s="147"/>
+      <c r="C52" s="153"/>
+      <c r="D52" s="154"/>
+      <c r="E52" s="154"/>
+      <c r="F52" s="154"/>
+      <c r="G52" s="154"/>
+      <c r="H52" s="154"/>
+      <c r="I52" s="154"/>
+      <c r="J52" s="154"/>
+      <c r="K52" s="154"/>
+      <c r="L52" s="154"/>
+      <c r="M52" s="154"/>
+      <c r="N52" s="154"/>
+      <c r="O52" s="155"/>
       <c r="Q52" s="55"/>
     </row>
     <row r="53" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B53" s="116"/>
-      <c r="C53" s="145"/>
-      <c r="D53" s="146"/>
-      <c r="E53" s="146"/>
-      <c r="F53" s="146"/>
-      <c r="G53" s="146"/>
-      <c r="H53" s="146"/>
-      <c r="I53" s="146"/>
-      <c r="J53" s="146"/>
-      <c r="K53" s="146"/>
-      <c r="L53" s="146"/>
-      <c r="M53" s="146"/>
-      <c r="N53" s="146"/>
-      <c r="O53" s="147"/>
+      <c r="C53" s="153"/>
+      <c r="D53" s="154"/>
+      <c r="E53" s="154"/>
+      <c r="F53" s="154"/>
+      <c r="G53" s="154"/>
+      <c r="H53" s="154"/>
+      <c r="I53" s="154"/>
+      <c r="J53" s="154"/>
+      <c r="K53" s="154"/>
+      <c r="L53" s="154"/>
+      <c r="M53" s="154"/>
+      <c r="N53" s="154"/>
+      <c r="O53" s="155"/>
       <c r="Q53" s="55"/>
     </row>
     <row r="54" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B54" s="116"/>
-      <c r="C54" s="145"/>
-      <c r="D54" s="146"/>
-      <c r="E54" s="146"/>
-      <c r="F54" s="146"/>
-      <c r="G54" s="146"/>
-      <c r="H54" s="146"/>
-      <c r="I54" s="146"/>
-      <c r="J54" s="146"/>
-      <c r="K54" s="146"/>
-      <c r="L54" s="146"/>
-      <c r="M54" s="146"/>
-      <c r="N54" s="146"/>
-      <c r="O54" s="147"/>
+      <c r="C54" s="153"/>
+      <c r="D54" s="154"/>
+      <c r="E54" s="154"/>
+      <c r="F54" s="154"/>
+      <c r="G54" s="154"/>
+      <c r="H54" s="154"/>
+      <c r="I54" s="154"/>
+      <c r="J54" s="154"/>
+      <c r="K54" s="154"/>
+      <c r="L54" s="154"/>
+      <c r="M54" s="154"/>
+      <c r="N54" s="154"/>
+      <c r="O54" s="155"/>
       <c r="Q54" s="55"/>
     </row>
     <row r="55" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
       <c r="B55" s="118"/>
-      <c r="C55" s="145"/>
-      <c r="D55" s="146"/>
-      <c r="E55" s="146"/>
-      <c r="F55" s="146"/>
-      <c r="G55" s="146"/>
-      <c r="H55" s="146"/>
-      <c r="I55" s="146"/>
-      <c r="J55" s="146"/>
-      <c r="K55" s="146"/>
-      <c r="L55" s="146"/>
-      <c r="M55" s="146"/>
-      <c r="N55" s="146"/>
-      <c r="O55" s="147"/>
+      <c r="C55" s="153"/>
+      <c r="D55" s="154"/>
+      <c r="E55" s="154"/>
+      <c r="F55" s="154"/>
+      <c r="G55" s="154"/>
+      <c r="H55" s="154"/>
+      <c r="I55" s="154"/>
+      <c r="J55" s="154"/>
+      <c r="K55" s="154"/>
+      <c r="L55" s="154"/>
+      <c r="M55" s="154"/>
+      <c r="N55" s="154"/>
+      <c r="O55" s="155"/>
       <c r="Q55" s="55"/>
     </row>
     <row r="56" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="10"/>
       <c r="B56" s="117"/>
-      <c r="C56" s="145"/>
-      <c r="D56" s="146"/>
-      <c r="E56" s="146"/>
-      <c r="F56" s="146"/>
-      <c r="G56" s="146"/>
-      <c r="H56" s="146"/>
-      <c r="I56" s="146"/>
-      <c r="J56" s="146"/>
-      <c r="K56" s="146"/>
-      <c r="L56" s="146"/>
-      <c r="M56" s="146"/>
-      <c r="N56" s="146"/>
-      <c r="O56" s="147"/>
+      <c r="C56" s="153"/>
+      <c r="D56" s="154"/>
+      <c r="E56" s="154"/>
+      <c r="F56" s="154"/>
+      <c r="G56" s="154"/>
+      <c r="H56" s="154"/>
+      <c r="I56" s="154"/>
+      <c r="J56" s="154"/>
+      <c r="K56" s="154"/>
+      <c r="L56" s="154"/>
+      <c r="M56" s="154"/>
+      <c r="N56" s="154"/>
+      <c r="O56" s="155"/>
       <c r="Q56" s="55"/>
     </row>
     <row r="57" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
@@ -13809,89 +13816,89 @@
     </row>
     <row r="60" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B60" s="116"/>
-      <c r="C60" s="145"/>
-      <c r="D60" s="146"/>
-      <c r="E60" s="146"/>
-      <c r="F60" s="146"/>
-      <c r="G60" s="146"/>
-      <c r="H60" s="146"/>
-      <c r="I60" s="146"/>
-      <c r="J60" s="146"/>
-      <c r="K60" s="146"/>
-      <c r="L60" s="146"/>
-      <c r="M60" s="146"/>
-      <c r="N60" s="146"/>
-      <c r="O60" s="147"/>
+      <c r="C60" s="153"/>
+      <c r="D60" s="154"/>
+      <c r="E60" s="154"/>
+      <c r="F60" s="154"/>
+      <c r="G60" s="154"/>
+      <c r="H60" s="154"/>
+      <c r="I60" s="154"/>
+      <c r="J60" s="154"/>
+      <c r="K60" s="154"/>
+      <c r="L60" s="154"/>
+      <c r="M60" s="154"/>
+      <c r="N60" s="154"/>
+      <c r="O60" s="155"/>
       <c r="Q60" s="55"/>
     </row>
     <row r="61" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B61" s="116"/>
-      <c r="C61" s="145"/>
-      <c r="D61" s="146"/>
-      <c r="E61" s="146"/>
-      <c r="F61" s="146"/>
-      <c r="G61" s="146"/>
-      <c r="H61" s="146"/>
-      <c r="I61" s="146"/>
-      <c r="J61" s="146"/>
-      <c r="K61" s="146"/>
-      <c r="L61" s="146"/>
-      <c r="M61" s="146"/>
-      <c r="N61" s="146"/>
-      <c r="O61" s="147"/>
+      <c r="C61" s="153"/>
+      <c r="D61" s="154"/>
+      <c r="E61" s="154"/>
+      <c r="F61" s="154"/>
+      <c r="G61" s="154"/>
+      <c r="H61" s="154"/>
+      <c r="I61" s="154"/>
+      <c r="J61" s="154"/>
+      <c r="K61" s="154"/>
+      <c r="L61" s="154"/>
+      <c r="M61" s="154"/>
+      <c r="N61" s="154"/>
+      <c r="O61" s="155"/>
       <c r="Q61" s="55"/>
     </row>
     <row r="62" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B62" s="116"/>
-      <c r="C62" s="145"/>
-      <c r="D62" s="146"/>
-      <c r="E62" s="146"/>
-      <c r="F62" s="146"/>
-      <c r="G62" s="146"/>
-      <c r="H62" s="146"/>
-      <c r="I62" s="146"/>
-      <c r="J62" s="146"/>
-      <c r="K62" s="146"/>
-      <c r="L62" s="146"/>
-      <c r="M62" s="146"/>
-      <c r="N62" s="146"/>
-      <c r="O62" s="147"/>
+      <c r="C62" s="153"/>
+      <c r="D62" s="154"/>
+      <c r="E62" s="154"/>
+      <c r="F62" s="154"/>
+      <c r="G62" s="154"/>
+      <c r="H62" s="154"/>
+      <c r="I62" s="154"/>
+      <c r="J62" s="154"/>
+      <c r="K62" s="154"/>
+      <c r="L62" s="154"/>
+      <c r="M62" s="154"/>
+      <c r="N62" s="154"/>
+      <c r="O62" s="155"/>
       <c r="Q62" s="55"/>
     </row>
     <row r="63" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6"/>
       <c r="B63" s="118"/>
-      <c r="C63" s="145"/>
-      <c r="D63" s="146"/>
-      <c r="E63" s="146"/>
-      <c r="F63" s="146"/>
-      <c r="G63" s="146"/>
-      <c r="H63" s="146"/>
-      <c r="I63" s="146"/>
-      <c r="J63" s="146"/>
-      <c r="K63" s="146"/>
-      <c r="L63" s="146"/>
-      <c r="M63" s="146"/>
-      <c r="N63" s="146"/>
-      <c r="O63" s="147"/>
+      <c r="C63" s="153"/>
+      <c r="D63" s="154"/>
+      <c r="E63" s="154"/>
+      <c r="F63" s="154"/>
+      <c r="G63" s="154"/>
+      <c r="H63" s="154"/>
+      <c r="I63" s="154"/>
+      <c r="J63" s="154"/>
+      <c r="K63" s="154"/>
+      <c r="L63" s="154"/>
+      <c r="M63" s="154"/>
+      <c r="N63" s="154"/>
+      <c r="O63" s="155"/>
       <c r="Q63" s="55"/>
     </row>
     <row r="64" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="10"/>
       <c r="B64" s="117"/>
-      <c r="C64" s="145"/>
-      <c r="D64" s="146"/>
-      <c r="E64" s="146"/>
-      <c r="F64" s="146"/>
-      <c r="G64" s="146"/>
-      <c r="H64" s="146"/>
-      <c r="I64" s="146"/>
-      <c r="J64" s="146"/>
-      <c r="K64" s="146"/>
-      <c r="L64" s="146"/>
-      <c r="M64" s="146"/>
-      <c r="N64" s="146"/>
-      <c r="O64" s="147"/>
+      <c r="C64" s="153"/>
+      <c r="D64" s="154"/>
+      <c r="E64" s="154"/>
+      <c r="F64" s="154"/>
+      <c r="G64" s="154"/>
+      <c r="H64" s="154"/>
+      <c r="I64" s="154"/>
+      <c r="J64" s="154"/>
+      <c r="K64" s="154"/>
+      <c r="L64" s="154"/>
+      <c r="M64" s="154"/>
+      <c r="N64" s="154"/>
+      <c r="O64" s="155"/>
       <c r="Q64" s="55"/>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.3">
@@ -13949,13 +13956,17 @@
     <sortCondition descending="1" ref="B60"/>
   </sortState>
   <mergeCells count="34">
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="B1:O1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="C60:O60"/>
+    <mergeCell ref="C61:O61"/>
+    <mergeCell ref="C62:O62"/>
+    <mergeCell ref="C63:O63"/>
+    <mergeCell ref="C64:O64"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="J17:O17"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="J29:O29"/>
     <mergeCell ref="B58:O58"/>
     <mergeCell ref="C59:O59"/>
     <mergeCell ref="B42:O42"/>
@@ -13972,17 +13983,13 @@
     <mergeCell ref="C54:O54"/>
     <mergeCell ref="C55:O55"/>
     <mergeCell ref="C56:O56"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="J17:O17"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="J29:O29"/>
-    <mergeCell ref="C60:O60"/>
-    <mergeCell ref="C61:O61"/>
-    <mergeCell ref="C62:O62"/>
-    <mergeCell ref="C63:O63"/>
-    <mergeCell ref="C64:O64"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="N2:O2"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -14045,7 +14052,7 @@
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="12"/>
@@ -14072,10 +14079,10 @@
       <c r="A7" s="59"/>
       <c r="B7" s="59"/>
       <c r="C7" s="113" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D7" s="159" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E7" s="159"/>
       <c r="F7" s="159"/>
@@ -14085,7 +14092,7 @@
       <c r="A8" s="59"/>
       <c r="B8" s="59"/>
       <c r="C8" s="113" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D8" s="160" t="s">
         <v>51</v>
@@ -14098,10 +14105,10 @@
       <c r="A9" s="59"/>
       <c r="B9" s="59"/>
       <c r="C9" s="113" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D9" s="159" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E9" s="160"/>
       <c r="F9" s="160"/>
@@ -14213,7 +14220,7 @@
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E21" s="120">
         <f ca="1">TODAY()</f>
-        <v>44308</v>
+        <v>44310</v>
       </c>
       <c r="F21" s="120"/>
     </row>
@@ -14240,10 +14247,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC76BB1-6D17-4F01-9A8C-BA89276F8B85}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14278,79 +14285,104 @@
     <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="54"/>
       <c r="B4" s="161" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C4" s="161"/>
       <c r="D4" s="54"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="54"/>
       <c r="B5" s="136">
         <v>1</v>
       </c>
       <c r="C5" s="137" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="D5" s="54"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="54"/>
-      <c r="B6" s="136">
-        <v>2</v>
-      </c>
-      <c r="C6" s="137" t="s">
-        <v>63</v>
-      </c>
+      <c r="B6" s="133"/>
+      <c r="C6" s="130"/>
       <c r="D6" s="54"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="54"/>
-      <c r="B7" s="136">
-        <v>3</v>
-      </c>
-      <c r="C7" s="137" t="s">
-        <v>60</v>
-      </c>
+      <c r="B7" s="161" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="161"/>
       <c r="D7" s="54"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="54"/>
       <c r="B8" s="136">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C8" s="137" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D8" s="54"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="54"/>
       <c r="B9" s="136">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C9" s="137" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="D9" s="54"/>
     </row>
-    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="54"/>
       <c r="B10" s="136">
+        <v>3</v>
+      </c>
+      <c r="C10" s="137" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="54"/>
+    </row>
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="54"/>
+      <c r="B11" s="136">
+        <v>4</v>
+      </c>
+      <c r="C11" s="137" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="54"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="54"/>
+      <c r="B12" s="136">
+        <v>5</v>
+      </c>
+      <c r="C12" s="137" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="54"/>
+    </row>
+    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="54"/>
+      <c r="B13" s="136">
         <v>6</v>
       </c>
-      <c r="C10" s="137" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="54"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="54"/>
-      <c r="B11" s="133"/>
-      <c r="C11" s="130"/>
-      <c r="D11" s="54"/>
+      <c r="C13" s="137" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="54"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="54"/>
+      <c r="B14" s="133"/>
+      <c r="C14" s="130"/>
+      <c r="D14" s="54"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14359,9 +14391,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14479,25 +14514,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B77CED7-C41E-49ED-87B0-E2E378B9D0FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DBF3B54-18FF-425E-9D16-518FEEB123AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -14519,9 +14544,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DBF3B54-18FF-425E-9D16-518FEEB123AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B77CED7-C41E-49ED-87B0-E2E378B9D0FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>